<commit_message>
Updated Scrum Board and Scrum Master log files
</commit_message>
<xml_diff>
--- a/Project/Work Breakdown Structure.xlsx
+++ b/Project/Work Breakdown Structure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruno\Desktop\JabRef\jabref\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB10C5A-27F8-4621-9931-CFFF60CAE420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A86EC8A-CC0E-4976-BC30-9B7090D08EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,10 +99,10 @@
     <t xml:space="preserve">Elaborate 1 sub use-case diagram </t>
   </si>
   <si>
-    <t>Identify a subset use-case withing the TOP use-case diagram</t>
-  </si>
-  <si>
     <t>(Team Effort) Elaborate TOP use-case diagram</t>
+  </si>
+  <si>
+    <t>Identify a subset use-case within the TOP use-case diagram</t>
   </si>
 </sst>
 </file>
@@ -629,7 +629,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +680,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>23</v>

</xml_diff>